<commit_message>
import button moved to counterparties
</commit_message>
<xml_diff>
--- a/src/main/resources/import_test_data/tc1.xlsx
+++ b/src/main/resources/import_test_data/tc1.xlsx
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -403,48 +403,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>50000</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>50000</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>200000</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>